<commit_message>
Muestra todas las gráficas
</commit_message>
<xml_diff>
--- a/Saberpro16.xlsx
+++ b/Saberpro16.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\VISUALIZACIÓN\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristian\Documents\visualizacion\Trabajo 1\visualizacion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="2016" sheetId="3" r:id="rId1"/>
@@ -404,7 +404,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
       <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
@@ -2974,26 +2974,11 @@
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
-        <f>SUM(A2:A80)/80</f>
-        <v>171.98750000000001</v>
-      </c>
-      <c r="C82" s="1">
-        <f>SUM(C2:C80)/80</f>
-        <v>154.75</v>
-      </c>
-      <c r="E82" s="1">
-        <f>SUM(E2:E80)/80</f>
-        <v>149.01249999999999</v>
-      </c>
-      <c r="G82" s="1">
-        <f>SUM(G2:G80)/80</f>
-        <v>158.25</v>
-      </c>
-      <c r="I82" s="1">
-        <f>SUM(I2:I80)/80</f>
-        <v>150.28749999999999</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="C82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="G82" s="1"/>
+      <c r="I82" s="1"/>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="1"/>
@@ -3007,7 +2992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
+    <sheetView topLeftCell="B59" workbookViewId="0">
       <selection activeCell="K69" sqref="K69"/>
     </sheetView>
   </sheetViews>
@@ -5301,7 +5286,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B61" workbookViewId="0">
       <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
@@ -7592,7 +7577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A85" workbookViewId="0">
       <selection activeCell="L89" sqref="L89"/>
     </sheetView>
   </sheetViews>

</xml_diff>